<commit_message>
write data in excel sheet
</commit_message>
<xml_diff>
--- a/Actitime/data/input.xlsx
+++ b/Actitime/data/input.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ValidLoginPage" sheetId="1" r:id="rId1"/>
     <sheet name="invalidLogin" sheetId="2" r:id="rId2"/>
     <sheet name="IssueDate" sheetId="3" r:id="rId3"/>
+    <sheet name="irctc" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>admin</t>
   </si>
@@ -55,13 +56,26 @@
   </si>
   <si>
     <t>Jul 14, 2017</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>phoneNo</t>
+  </si>
+  <si>
+    <t>New Delhi</t>
+  </si>
+  <si>
+    <t>: 011-23221147</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,6 +85,20 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -117,12 +145,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,8 +462,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -473,7 +503,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -522,14 +552,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -558,4 +588,36 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>